<commit_message>
- Ignores sheets which name starts with a exclamation mark (!) - Ignores empty sheets
</commit_message>
<xml_diff>
--- a/samples/SampleBook.xlsx
+++ b/samples/SampleBook.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="13110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="1" r:id="rId1"/>
     <sheet name="Second" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="!Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>a</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>!a</t>
+  </si>
+  <si>
+    <t>Tach</t>
+  </si>
+  <si>
+    <t>Moin</t>
   </si>
 </sst>
 </file>
@@ -577,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1038,12 +1044,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>